<commit_message>
refs #660 Risiken 1-4
</commit_message>
<xml_diff>
--- a/doc/Bericht/05_Technischer Bericht/02_Projektmanagement/Risikomanagement.xlsx
+++ b/doc/Bericht/05_Technischer Bericht/02_Projektmanagement/Risikomanagement.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="225" windowWidth="11640" windowHeight="5400" activeTab="1"/>
+    <workbookView xWindow="-15" yWindow="30" windowWidth="12390" windowHeight="11955" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Änderungsgeschichte" sheetId="3" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>Risikomanagement</t>
   </si>
@@ -62,60 +62,9 @@
     <t>Autor</t>
   </si>
   <si>
-    <t>dtreichl</t>
-  </si>
-  <si>
-    <t>Surface2 wird nicht rechtzeitig geliefert</t>
-  </si>
-  <si>
-    <t>Einarbeitung Surface</t>
-  </si>
-  <si>
-    <t>Michael Gfeller hat bereits Erfahrung mit Surface. Bei allfälligen Problemen kann und soll er um Rat angefragt werden.</t>
-  </si>
-  <si>
-    <t>Die Einarbeitung in Surface benötigt mehr Zeit als ursprünglich geplant.</t>
-  </si>
-  <si>
-    <t>Der Touchtisch kann nicht rechtzeitig geliefert werden. Somit ist das Testen von Touch und Tags etc. nicht möglich.</t>
-  </si>
-  <si>
     <t>Konzentration auf die wichtigsten Kernfunktionalitäten, ev. werden gewisse Funktionen weggelassen.</t>
   </si>
   <si>
-    <t>Der Funktionsumfang des Projektes wird wenn nötig reduziert.</t>
-  </si>
-  <si>
-    <t>PDF auf Surface darstellen kompliziert</t>
-  </si>
-  <si>
-    <t>Es ist kompliziert, ein PDF auf dem Surface darzustellen. Möglicherweise muss das PDF Dokument in ein anderes Format umgewandelt werden.</t>
-  </si>
-  <si>
-    <t>Das Problem wir früh angegangen und bereits im Architekturprototypen umgesetzt.</t>
-  </si>
-  <si>
-    <t>lemer</t>
-  </si>
-  <si>
-    <t>Umwandlung in anderen Dokumenttypen wird programmiert oder externe Hilfe wird angefordert.</t>
-  </si>
-  <si>
-    <t>lelmer</t>
-  </si>
-  <si>
-    <t>Review</t>
-  </si>
-  <si>
-    <t>cheidt</t>
-  </si>
-  <si>
-    <t>Alternative Testmethoden nutzen, um Testumgebung zu simulieren.</t>
-  </si>
-  <si>
-    <t>Keine, nicht möglich.</t>
-  </si>
-  <si>
     <t>Nr.</t>
   </si>
   <si>
@@ -128,43 +77,52 @@
     <t>Schadens-potenzial [h]</t>
   </si>
   <si>
-    <t>R4 bereinigt</t>
-  </si>
-  <si>
-    <t>Neues Risiko R5 gemäss Skype-Meeting</t>
-  </si>
-  <si>
-    <t>Neues Risiko R6</t>
-  </si>
-  <si>
-    <t>Neues Risiko R7, R2 Wahrscheinlichkeit von 20% auf 15% angepasst.</t>
-  </si>
-  <si>
-    <t>R1, R6 sind eingetreten und somit bereinigt, R2 ist mit den User Stories wahrscheinlicher geworden, Layout angepasst.</t>
-  </si>
-  <si>
-    <t>R7 bereinigt</t>
-  </si>
-  <si>
-    <t>Schadenspotenzial R2 angepasst, R3 bereinigt</t>
-  </si>
-  <si>
-    <t>keine Nachführung nötig gewesen</t>
-  </si>
-  <si>
-    <t>R2 bereinigt, keine Risiken mehr vorhanden</t>
-  </si>
-  <si>
     <t>Sprint neu</t>
   </si>
   <si>
     <t>Sprint bereinigt</t>
   </si>
   <si>
-    <t>R4 hinzugefügt + Werte angepasst</t>
-  </si>
-  <si>
     <t>Fehlein-schätzung des Zeitaufwands</t>
+  </si>
+  <si>
+    <t>Endgültige Hardware wird nicht rechtzeitig geliefert</t>
+  </si>
+  <si>
+    <t>Keine</t>
+  </si>
+  <si>
+    <t>Es wird ein alternatives Testsetup erarbeitet, mithilfe dessen die Arbeit getestet werden kann.</t>
+  </si>
+  <si>
+    <t>DT</t>
+  </si>
+  <si>
+    <t>Die Hardware für die Video Wall kann nicht   rechtzeitig geliefert werden.</t>
+  </si>
+  <si>
+    <t>Auflösung der Video Wall ungenügend</t>
+  </si>
+  <si>
+    <t>Die Auflösung der Video Wall ist für das Lesen der Bachelor Posters ungenügend</t>
+  </si>
+  <si>
+    <t>Suchen einer Lösung für die Erstellung der Video Wall, bei der jeder einzelne Monitor Full HD ist.</t>
+  </si>
+  <si>
+    <t>Darstellung der Posters in einer Grösse, die am besten lesbar ist.</t>
+  </si>
+  <si>
+    <t>Kinect erkennt Ausrichtung nicht</t>
+  </si>
+  <si>
+    <t>Kinect erkennt die seitliche Ausrichtung des Körpers der sich vor der Video Wall befindlichen Person nicht.</t>
+  </si>
+  <si>
+    <t>Testen der Erkennung der Ausrichtung mit vorhandenen Frameworks.</t>
+  </si>
+  <si>
+    <t>Es wird das Framework verwendet, welches die Position/Ausrichtung am besten erkennt. Da drei Frameworks zur Verfügung stehen ist die Wahrscheinlichkeit des Eintreffens dieses Risikos eher klein einzuschätzen.</t>
   </si>
 </sst>
 </file>
@@ -256,7 +214,7 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -276,32 +234,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -312,6 +258,95 @@
     <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="36">
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -388,105 +423,16 @@
         </horizontal>
       </border>
     </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium5 2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="TableStyleMedium5 2" pivot="0" count="7">
-      <tableStyleElement type="wholeTable" dxfId="6"/>
-      <tableStyleElement type="headerRow" dxfId="5"/>
-      <tableStyleElement type="totalRow" dxfId="4"/>
-      <tableStyleElement type="firstColumn" dxfId="3"/>
-      <tableStyleElement type="lastColumn" dxfId="2"/>
-      <tableStyleElement type="firstRowStripe" dxfId="1"/>
-      <tableStyleElement type="firstColumnStripe" dxfId="0"/>
+      <tableStyleElement type="wholeTable" dxfId="35"/>
+      <tableStyleElement type="headerRow" dxfId="34"/>
+      <tableStyleElement type="totalRow" dxfId="33"/>
+      <tableStyleElement type="firstColumn" dxfId="32"/>
+      <tableStyleElement type="lastColumn" dxfId="31"/>
+      <tableStyleElement type="firstRowStripe" dxfId="30"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="29"/>
     </tableStyle>
   </tableStyles>
   <colors>
@@ -509,30 +455,30 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A3:D15" totalsRowShown="0" headerRowDxfId="35" dataDxfId="34">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A3:D4" totalsRowShown="0" headerRowDxfId="28" dataDxfId="27">
   <tableColumns count="4">
-    <tableColumn id="1" name="Datum" dataDxfId="33"/>
-    <tableColumn id="2" name="Version" dataDxfId="32"/>
-    <tableColumn id="3" name="Änderung" dataDxfId="31"/>
-    <tableColumn id="5" name="Autor" dataDxfId="30"/>
+    <tableColumn id="1" name="Datum" dataDxfId="26"/>
+    <tableColumn id="2" name="Version" dataDxfId="25"/>
+    <tableColumn id="3" name="Änderung" dataDxfId="24"/>
+    <tableColumn id="5" name="Autor" dataDxfId="23"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium5 2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A3:J9" totalsRowCount="1" headerRowDxfId="9" dataDxfId="8" totalsRowDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A3:J9" totalsRowCount="1" headerRowDxfId="22" dataDxfId="21" totalsRowDxfId="20">
   <tableColumns count="10">
-    <tableColumn id="1" name="Nr." totalsRowLabel="Total" dataDxfId="29" totalsRowDxfId="28"/>
-    <tableColumn id="2" name="Risiko" dataDxfId="27" totalsRowDxfId="26"/>
-    <tableColumn id="3" name="Beschreibung" dataDxfId="25" totalsRowDxfId="24"/>
-    <tableColumn id="4" name="W'keit des Eintretens [%]" dataDxfId="23" totalsRowDxfId="22"/>
-    <tableColumn id="5" name="Schadens-potenzial [h]" totalsRowFunction="sum" dataDxfId="21" totalsRowDxfId="20"/>
-    <tableColumn id="6" name="Reserven [h]" totalsRowFunction="sum" dataDxfId="19" totalsRowDxfId="18"/>
-    <tableColumn id="7" name="Vermeidungs- und Verminderungsmassnahmen" dataDxfId="17" totalsRowDxfId="16"/>
-    <tableColumn id="8" name="Aktionen beim Eintreffen" dataDxfId="15" totalsRowDxfId="14"/>
-    <tableColumn id="10" name="Sprint neu" dataDxfId="13" totalsRowDxfId="12"/>
-    <tableColumn id="11" name="Sprint bereinigt" dataDxfId="11" totalsRowDxfId="10"/>
+    <tableColumn id="1" name="Nr." totalsRowLabel="Total" dataDxfId="19" totalsRowDxfId="9"/>
+    <tableColumn id="2" name="Risiko" dataDxfId="18" totalsRowDxfId="8"/>
+    <tableColumn id="3" name="Beschreibung" dataDxfId="17" totalsRowDxfId="7"/>
+    <tableColumn id="4" name="W'keit des Eintretens [%]" dataDxfId="16" totalsRowDxfId="6"/>
+    <tableColumn id="5" name="Schadens-potenzial [h]" totalsRowFunction="sum" dataDxfId="15" totalsRowDxfId="5"/>
+    <tableColumn id="6" name="Reserven [h]" totalsRowFunction="sum" dataDxfId="14" totalsRowDxfId="4"/>
+    <tableColumn id="7" name="Vermeidungs- und Verminderungsmassnahmen" dataDxfId="13" totalsRowDxfId="3"/>
+    <tableColumn id="8" name="Aktionen beim Eintreffen" dataDxfId="12" totalsRowDxfId="2"/>
+    <tableColumn id="10" name="Sprint neu" dataDxfId="11" totalsRowDxfId="1"/>
+    <tableColumn id="11" name="Sprint bereinigt" dataDxfId="10" totalsRowDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium5 2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -825,10 +771,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -839,21 +785,27 @@
     <col min="4" max="4" width="8.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="22.5" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:10" ht="22.5" x14ac:dyDescent="0.3">
+      <c r="A1" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
+      <c r="J1" s="10"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>6</v>
       </c>
@@ -867,175 +819,24 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="9">
-        <v>40809</v>
-      </c>
-      <c r="B4" s="13">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="8">
+        <v>40962</v>
+      </c>
+      <c r="B4" s="9">
         <v>1</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>10</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="9">
-        <v>40811</v>
-      </c>
-      <c r="B5" s="13">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="D5" s="5" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="9">
-        <v>40811</v>
-      </c>
-      <c r="B6" s="13">
-        <v>1.2</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="9">
-        <v>40816</v>
-      </c>
-      <c r="B7" s="13">
-        <v>1.3</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="9">
-        <v>40819</v>
-      </c>
-      <c r="B8" s="13">
-        <v>1.4</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="9">
-        <v>37180</v>
-      </c>
-      <c r="B9" s="13">
-        <v>1.5</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="9">
-        <v>40833</v>
-      </c>
-      <c r="B10" s="13">
-        <v>1.6</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="10">
-        <v>40839</v>
-      </c>
-      <c r="B11" s="14">
-        <v>1.7</v>
-      </c>
-      <c r="C11" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="10">
-        <v>40847</v>
-      </c>
-      <c r="B12" s="14">
-        <v>1.8</v>
-      </c>
-      <c r="C12" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="10">
-        <v>40861</v>
-      </c>
-      <c r="B13" s="14">
-        <v>1.9</v>
-      </c>
-      <c r="C13" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="10">
-        <v>40875</v>
-      </c>
-      <c r="B14" s="12">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="C14" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="10">
-        <v>40890</v>
-      </c>
-      <c r="B15" s="12">
-        <v>1.1100000000000001</v>
-      </c>
-      <c r="C15" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:D1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
   <tableParts count="1">
@@ -1050,7 +851,7 @@
   <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1068,22 +869,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="22.5" x14ac:dyDescent="0.3">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="15"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="12"/>
     </row>
     <row r="3" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>32</v>
+        <v>15</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>1</v>
@@ -1091,13 +892,13 @@
       <c r="C3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="F3" s="8" t="s">
+      <c r="D3" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="7" t="s">
         <v>3</v>
       </c>
       <c r="G3" s="4" t="s">
@@ -1107,24 +908,24 @@
         <v>5</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>45</v>
+        <v>19</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="90" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>1</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="D4" s="4">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="E4" s="4">
         <v>0</v>
@@ -1133,116 +934,108 @@
         <v>0</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="I4" s="4">
-        <v>1</v>
-      </c>
-      <c r="J4" s="4">
-        <v>2</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="J4" s="4"/>
     </row>
     <row r="5" spans="1:10" ht="165" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>2</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>48</v>
+        <v>21</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>12</v>
       </c>
       <c r="D5" s="4">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="E5" s="4">
         <v>20</v>
       </c>
       <c r="F5" s="4">
         <f t="shared" ref="F5:F7" si="0">(D5/100)*E5</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>11</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="I5" s="4">
-        <v>1</v>
-      </c>
-      <c r="J5" s="4">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="105" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="J5" s="4"/>
+    </row>
+    <row r="6" spans="1:10" ht="165" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>3</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>18</v>
+        <v>32</v>
       </c>
       <c r="D6" s="4">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="E6" s="4">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="F6" s="4">
         <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="I6" s="4">
         <v>0</v>
       </c>
-      <c r="G6" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="I6" s="4">
-        <v>1</v>
-      </c>
-      <c r="J6" s="4">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="135" x14ac:dyDescent="0.25">
+      <c r="J6" s="4"/>
+    </row>
+    <row r="7" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>4</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="D7" s="4">
+        <v>30</v>
+      </c>
+      <c r="E7" s="4">
         <v>0</v>
-      </c>
-      <c r="E7" s="4">
-        <v>50</v>
       </c>
       <c r="F7" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="I7" s="4">
-        <v>1</v>
-      </c>
-      <c r="J7" s="4">
-        <v>1</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="J7" s="4"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
@@ -1258,18 +1051,18 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>34</v>
+        <v>17</v>
       </c>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
       <c r="E9" s="4">
         <f>SUBTOTAL(109,Table1[Schadens-potenzial '[h']])</f>
-        <v>120</v>
+        <v>40</v>
       </c>
       <c r="F9" s="4">
         <f>SUBTOTAL(109,Table1[Reserven '[h']])</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G9" s="4"/>
       <c r="H9" s="4"/>

</xml_diff>

<commit_message>
refs #672 Review des Risikomanagements
</commit_message>
<xml_diff>
--- a/doc/Bericht/05_Technischer Bericht/02_Projektmanagement/Risikomanagement.xlsx
+++ b/doc/Bericht/05_Technischer Bericht/02_Projektmanagement/Risikomanagement.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="53">
   <si>
     <t>Risikomanagement</t>
   </si>
@@ -89,24 +89,15 @@
     <t>DT</t>
   </si>
   <si>
-    <t>Die Hardware für die Video Wall kann nicht   rechtzeitig geliefert werden.</t>
-  </si>
-  <si>
     <t>Auflösung der Video Wall ungenügend</t>
   </si>
   <si>
-    <t>Die Auflösung der Video Wall ist für das Lesen der Bachelor Posters ungenügend</t>
-  </si>
-  <si>
     <t>Suchen einer Lösung für die Erstellung der Video Wall, bei der jeder einzelne Monitor Full HD ist.</t>
   </si>
   <si>
     <t>Frühe Anfrage, frühe Abklärungen durch Markus Stolze / Schulleitung.</t>
   </si>
   <si>
-    <t>Scrum, Früher Prototyp, kleine Demoprogramme zu Beginn des Projektes. Kontinuierliche Überprüfung der Projektplanung und eventuelle Anpassung. Verantwortung für aktuellen Projektplan an einem Teammitglied zuweisen.</t>
-  </si>
-  <si>
     <t>Kinect: Seitliche Erkennung</t>
   </si>
   <si>
@@ -161,17 +152,32 @@
     <t>LE</t>
   </si>
   <si>
-    <t>Darstellung der Posters in einer Grösse, die gut lesbar ist. Usability Tests müssen wiederholt werden. Alternative (2h Aufwand): Zu kleine Texte / Dokumente dürfen nicht hochgeladen / angezeigt werden (Constraint einführen).</t>
-  </si>
-  <si>
-    <t>Risiko 1 ist eingetreten: HW wird nicht rechtzeitig geliefert. Deshalb muss alternatives Testsetup evaluiert (Schaden: 25h).
+    <t>Auf neue Risiken geprüft, leichte Anpassung an der Eintrittswahrscheinlichkeit vom Riskio 5, da laut Matrox eine Auflösung von mehr als FullHD pro Monitorausgang möglich ist.</t>
+  </si>
+  <si>
+    <t>1.2</t>
+  </si>
+  <si>
+    <t>Die Hardware für die Video Wall kann nicht  rechtzeitig geliefert werden.</t>
+  </si>
+  <si>
+    <t>Risiko 1 ist eingetreten: HW wird nicht rechtzeitig geliefert. Deshalb muss alternatives Testsetup evaluiert werden (Schaden: 25h).
 Neue Risiken hinzugefügt (4,6,7), Schätzungen angepasst, Beschreibungen erweitert</t>
   </si>
   <si>
-    <t>Auf neue Risiken geprüft, leichte Anpassung an der Eintrittswahrscheinlichkeit vom Riskio 5, da laut Matrox eine Auflösung von mehr als FullHD pro Monitorausgang möglich ist.</t>
-  </si>
-  <si>
-    <t>1.2</t>
+    <t>Scrum, früher Prototyp, kleine Demoprogramme zu Beginn des Projektes. Kontinuierliche Überprüfung der Projektplanung und eventuelle Anpassung. Verantwortung für aktuellen Projektplan an einem Teammitglied zuweisen.</t>
+  </si>
+  <si>
+    <t>Die Auflösung der Video Wall ist für das Lesen der Bachelor Posters ungenügend.</t>
+  </si>
+  <si>
+    <t>Darstellung der Poster in einer Grösse, die gut lesbar ist. Usability Tests müssen wiederholt werden. Alternative (2h Aufwand): Zu kleine Texte / Dokumente dürfen nicht hochgeladen / angezeigt werden (Constraint einführen).</t>
+  </si>
+  <si>
+    <t>1.3</t>
+  </si>
+  <si>
+    <t>Review, grammatikalische Korrekturen</t>
   </si>
 </sst>
 </file>
@@ -323,10 +329,10 @@
     </xf>
   </cellXfs>
   <cellStyles count="4">
-    <cellStyle name="20 % - Akzent4" xfId="3" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="Akzent4" xfId="2" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
-    <cellStyle name="Überschrift" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="3" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="2" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="36">
     <dxf>
@@ -526,7 +532,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A3:D6" totalsRowShown="0" headerRowDxfId="28" dataDxfId="27">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A3:D7" totalsRowShown="0" headerRowDxfId="28" dataDxfId="27">
   <tableColumns count="4">
     <tableColumn id="1" name="Datum" dataDxfId="26"/>
     <tableColumn id="2" name="Version" dataDxfId="25"/>
@@ -556,9 +562,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Larissa">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -596,7 +602,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Larissa">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -668,7 +674,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Larissa">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -842,13 +848,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.5703125" customWidth="1"/>
     <col min="2" max="2" width="10.140625" style="17" bestFit="1" customWidth="1"/>
@@ -895,7 +901,7 @@
         <v>40962</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>10</v>
@@ -912,10 +918,10 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -923,13 +929,27 @@
         <v>40970</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>46</v>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="11">
+        <v>40970</v>
+      </c>
+      <c r="B7" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -949,11 +969,11 @@
   <sheetPr codeName="Tabelle2"/>
   <dimension ref="A1:K17"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.42578125" customWidth="1"/>
     <col min="2" max="2" width="14.7109375" customWidth="1"/>
@@ -1022,7 +1042,7 @@
         <v>21</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>23</v>
+        <v>46</v>
       </c>
       <c r="D4" s="4">
         <v>100</v>
@@ -1035,10 +1055,10 @@
         <v>25</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="I4" s="4">
         <v>1</v>
@@ -1068,7 +1088,7 @@
         <v>5</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>28</v>
+        <v>48</v>
       </c>
       <c r="H5" s="4" t="s">
         <v>13</v>
@@ -1083,10 +1103,10 @@
         <v>3</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D6" s="4">
         <v>5</v>
@@ -1099,10 +1119,10 @@
         <v>4.5</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="I6" s="4">
         <v>1</v>
@@ -1114,10 +1134,10 @@
         <v>4</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D7" s="4">
         <v>15</v>
@@ -1130,13 +1150,13 @@
         <v>4.5</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="I7" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J7" s="4"/>
     </row>
@@ -1145,10 +1165,10 @@
         <v>5</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>25</v>
+        <v>49</v>
       </c>
       <c r="D8" s="4">
         <v>5</v>
@@ -1161,10 +1181,10 @@
         <v>3</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="I8" s="4">
         <v>1</v>
@@ -1176,10 +1196,10 @@
         <v>6</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D9" s="4">
         <v>30</v>
@@ -1192,10 +1212,10 @@
         <v>6</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="I9" s="4">
         <v>2</v>
@@ -1207,10 +1227,10 @@
         <v>7</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D10" s="4">
         <v>10</v>
@@ -1223,10 +1243,10 @@
         <v>6</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="I10" s="4">
         <v>2</v>

</xml_diff>

<commit_message>
refs #737 Dokumentation Kinectaufnahmen Geb. 4
Former-commit-id: d8e13f33a1614a88dad826d6e3e695bbca050249
</commit_message>
<xml_diff>
--- a/doc/Bericht/05_Technischer Bericht/02_Projektmanagement/Risikomanagement.xlsx
+++ b/doc/Bericht/05_Technischer Bericht/02_Projektmanagement/Risikomanagement.xlsx
@@ -98,12 +98,6 @@
     <t>Frühe Anfrage, frühe Abklärungen durch Markus Stolze / Schulleitung.</t>
   </si>
   <si>
-    <t>Kinect: Seitliche Erkennung</t>
-  </si>
-  <si>
-    <t>Kinect erkennt Menschen nicht, die sich seitlich vor der Video Wall bewegen.</t>
-  </si>
-  <si>
     <t>Kinect: Menschliche Drehung</t>
   </si>
   <si>
@@ -186,10 +180,16 @@
     <t>Review, keine Änderungen an den Risiken</t>
   </si>
   <si>
-    <t>Risiko 3 ist bereinigt durch die Aufnahmen, die mit Kinect im Gebäude 4 durchgeführt wurden.</t>
-  </si>
-  <si>
     <t>1.5</t>
+  </si>
+  <si>
+    <t>Kinect erkennt Menschen nicht, die sich parallel zur Wand ausgerichtet vor der Video Wall bewegen.</t>
+  </si>
+  <si>
+    <t>Kinect: Erkennung von der Seite</t>
+  </si>
+  <si>
+    <t>Risiko 3: "Kinect: Erkennung von der Seite" ist bereinigt durch die Aufnahmen, die mit Kinect im Gebäude 4 durchgeführt wurden (siehe Dokument Vorstudie).</t>
   </si>
 </sst>
 </file>
@@ -558,16 +558,16 @@
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A3:J12" totalsRowCount="1" headerRowDxfId="22" dataDxfId="21" totalsRowDxfId="20">
   <tableColumns count="10">
-    <tableColumn id="1" name="Nr." totalsRowLabel="Total" dataDxfId="19" totalsRowDxfId="9"/>
-    <tableColumn id="2" name="Risiko" dataDxfId="18" totalsRowDxfId="8"/>
-    <tableColumn id="3" name="Beschreibung" dataDxfId="17" totalsRowDxfId="7"/>
-    <tableColumn id="4" name="W'keit des Eintretens [%]" dataDxfId="16" totalsRowDxfId="6"/>
-    <tableColumn id="5" name="Schadens-potenzial [h]" totalsRowFunction="sum" dataDxfId="15" totalsRowDxfId="5"/>
-    <tableColumn id="6" name="Reserven [h]" totalsRowFunction="sum" dataDxfId="14" totalsRowDxfId="4"/>
-    <tableColumn id="7" name="Vermeidungs- und Verminderungsmassnahmen" dataDxfId="13" totalsRowDxfId="3"/>
-    <tableColumn id="8" name="Aktionen beim Eintreffen" dataDxfId="12" totalsRowDxfId="2"/>
-    <tableColumn id="10" name="Sprint neu" dataDxfId="11" totalsRowDxfId="1"/>
-    <tableColumn id="11" name="Sprint bereinigt" dataDxfId="10" totalsRowDxfId="0"/>
+    <tableColumn id="1" name="Nr." totalsRowLabel="Total" dataDxfId="19" totalsRowDxfId="18"/>
+    <tableColumn id="2" name="Risiko" dataDxfId="17" totalsRowDxfId="16"/>
+    <tableColumn id="3" name="Beschreibung" dataDxfId="15" totalsRowDxfId="14"/>
+    <tableColumn id="4" name="W'keit des Eintretens [%]" dataDxfId="13" totalsRowDxfId="12"/>
+    <tableColumn id="5" name="Schadens-potenzial [h]" totalsRowFunction="sum" dataDxfId="11" totalsRowDxfId="10"/>
+    <tableColumn id="6" name="Reserven [h]" totalsRowFunction="sum" dataDxfId="9" totalsRowDxfId="8"/>
+    <tableColumn id="7" name="Vermeidungs- und Verminderungsmassnahmen" dataDxfId="7" totalsRowDxfId="6"/>
+    <tableColumn id="8" name="Aktionen beim Eintreffen" dataDxfId="5" totalsRowDxfId="4"/>
+    <tableColumn id="10" name="Sprint neu" dataDxfId="3" totalsRowDxfId="2"/>
+    <tableColumn id="11" name="Sprint bereinigt" dataDxfId="1" totalsRowDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium5 2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -863,7 +863,7 @@
   <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -913,7 +913,7 @@
         <v>40962</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>10</v>
@@ -930,10 +930,10 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -941,13 +941,13 @@
         <v>40970</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -955,10 +955,10 @@
         <v>40970</v>
       </c>
       <c r="B7" s="16" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>22</v>
@@ -969,24 +969,24 @@
         <v>40976</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="11">
         <v>40984</v>
       </c>
       <c r="B9" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="C9" s="12" t="s">
         <v>56</v>
-      </c>
-      <c r="C9" s="12" t="s">
-        <v>55</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>22</v>
@@ -1010,7 +1010,7 @@
   <dimension ref="A1:K17"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1082,7 +1082,7 @@
         <v>21</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D4" s="4">
         <v>100</v>
@@ -1098,7 +1098,7 @@
         <v>25</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="I4" s="4">
         <v>1</v>
@@ -1128,7 +1128,7 @@
         <v>5</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="H5" s="4" t="s">
         <v>13</v>
@@ -1143,10 +1143,10 @@
         <v>3</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>26</v>
+        <v>55</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>27</v>
+        <v>54</v>
       </c>
       <c r="D6" s="4">
         <v>5</v>
@@ -1159,10 +1159,10 @@
         <v>4.5</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="I6" s="4">
         <v>1</v>
@@ -1176,10 +1176,10 @@
         <v>4</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D7" s="4">
         <v>15</v>
@@ -1192,10 +1192,10 @@
         <v>4.5</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="I7" s="4">
         <v>2</v>
@@ -1210,7 +1210,7 @@
         <v>23</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D8" s="4">
         <v>5</v>
@@ -1226,7 +1226,7 @@
         <v>24</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="I8" s="4">
         <v>1</v>
@@ -1238,10 +1238,10 @@
         <v>6</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D9" s="4">
         <v>30</v>
@@ -1254,10 +1254,10 @@
         <v>6</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="I9" s="4">
         <v>2</v>
@@ -1269,10 +1269,10 @@
         <v>7</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D10" s="4">
         <v>10</v>
@@ -1285,10 +1285,10 @@
         <v>6</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="I10" s="4">
         <v>2</v>

</xml_diff>

<commit_message>
refs #736 Korrekturen Markus refs #681 Erweiterung: Probleme mit Applikationen über die ganze Auflösung
Former-commit-id: 660e29abdf6915ff01e322a91b6fe183e6ce5711
</commit_message>
<xml_diff>
--- a/doc/Bericht/05_Technischer Bericht/02_Projektmanagement/Risikomanagement.xlsx
+++ b/doc/Bericht/05_Technischer Bericht/02_Projektmanagement/Risikomanagement.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="30" windowWidth="12390" windowHeight="11955"/>
+    <workbookView xWindow="-15" yWindow="30" windowWidth="12390" windowHeight="11955" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Änderungsgeschichte" sheetId="3" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="59">
   <si>
     <t>Risikomanagement</t>
   </si>
@@ -190,6 +190,12 @@
   </si>
   <si>
     <t>Risiko 3: "Kinect: Erkennung von der Seite" ist bereinigt durch die Aufnahmen, die mit Kinect im Gebäude 4 durchgeführt wurden (siehe Dokument Vorstudie).</t>
+  </si>
+  <si>
+    <t>WPF Applikationen laufen bei hoher Auflösung nicht flüssig</t>
+  </si>
+  <si>
+    <t>Die Applikation besitzt zwar die Wunschauflösung, diese ist aber dadurch sind Animationen nicht mehr flüssig und die Applikation stürzt im schlimmsten Fall ab.</t>
   </si>
 </sst>
 </file>
@@ -558,16 +564,16 @@
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A3:J12" totalsRowCount="1" headerRowDxfId="22" dataDxfId="21" totalsRowDxfId="20">
   <tableColumns count="10">
-    <tableColumn id="1" name="Nr." totalsRowLabel="Total" dataDxfId="19" totalsRowDxfId="18"/>
-    <tableColumn id="2" name="Risiko" dataDxfId="17" totalsRowDxfId="16"/>
-    <tableColumn id="3" name="Beschreibung" dataDxfId="15" totalsRowDxfId="14"/>
-    <tableColumn id="4" name="W'keit des Eintretens [%]" dataDxfId="13" totalsRowDxfId="12"/>
-    <tableColumn id="5" name="Schadens-potenzial [h]" totalsRowFunction="sum" dataDxfId="11" totalsRowDxfId="10"/>
-    <tableColumn id="6" name="Reserven [h]" totalsRowFunction="sum" dataDxfId="9" totalsRowDxfId="8"/>
-    <tableColumn id="7" name="Vermeidungs- und Verminderungsmassnahmen" dataDxfId="7" totalsRowDxfId="6"/>
-    <tableColumn id="8" name="Aktionen beim Eintreffen" dataDxfId="5" totalsRowDxfId="4"/>
-    <tableColumn id="10" name="Sprint neu" dataDxfId="3" totalsRowDxfId="2"/>
-    <tableColumn id="11" name="Sprint bereinigt" dataDxfId="1" totalsRowDxfId="0"/>
+    <tableColumn id="1" name="Nr." totalsRowLabel="Total" dataDxfId="19" totalsRowDxfId="9"/>
+    <tableColumn id="2" name="Risiko" dataDxfId="18" totalsRowDxfId="8"/>
+    <tableColumn id="3" name="Beschreibung" dataDxfId="17" totalsRowDxfId="7"/>
+    <tableColumn id="4" name="W'keit des Eintretens [%]" dataDxfId="16" totalsRowDxfId="6"/>
+    <tableColumn id="5" name="Schadens-potenzial [h]" totalsRowFunction="sum" dataDxfId="15" totalsRowDxfId="5"/>
+    <tableColumn id="6" name="Reserven [h]" totalsRowFunction="sum" dataDxfId="14" totalsRowDxfId="4"/>
+    <tableColumn id="7" name="Vermeidungs- und Verminderungsmassnahmen" dataDxfId="13" totalsRowDxfId="3"/>
+    <tableColumn id="8" name="Aktionen beim Eintreffen" dataDxfId="12" totalsRowDxfId="2"/>
+    <tableColumn id="10" name="Sprint neu" dataDxfId="11" totalsRowDxfId="1"/>
+    <tableColumn id="11" name="Sprint bereinigt" dataDxfId="10" totalsRowDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium5 2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -862,7 +868,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
@@ -1009,8 +1015,8 @@
   <sheetPr codeName="Tabelle2"/>
   <dimension ref="A1:K17"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1295,10 +1301,16 @@
       </c>
       <c r="J10" s="4"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="4"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
+    <row r="11" spans="1:10" ht="90" x14ac:dyDescent="0.25">
+      <c r="A11" s="4">
+        <v>8</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>58</v>
+      </c>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>

</xml_diff>

<commit_message>
refs #684 Risiko 4 bereinigt
Former-commit-id: 47de9416527845507c66f06d2b0e3eaa321d6a40
</commit_message>
<xml_diff>
--- a/doc/Bericht/05_Technischer Bericht/02_Projektmanagement/Risikomanagement.xlsx
+++ b/doc/Bericht/05_Technischer Bericht/02_Projektmanagement/Risikomanagement.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="30" windowWidth="12390" windowHeight="11955"/>
+    <workbookView xWindow="-15" yWindow="30" windowWidth="12390" windowHeight="11955" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Änderungsgeschichte" sheetId="3" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="67">
   <si>
     <t>Risikomanagement</t>
   </si>
@@ -214,6 +214,12 @@
   </si>
   <si>
     <t>Testen, ob tiefere Auflösung auch funktionieren würde. Applikation entsprechend so programmieren, dass sie auch mit einer tieferer Auflösung funktionieren würde. Dadurch wird das Schadenspotzenzial auch viel tiefer; dies wäre ohne diese Massnahme viel grösser, da die App umprogrammiert werden müsste. Eingesetzte Zeit, um das Risiko zu vermeiden: 8h.</t>
+  </si>
+  <si>
+    <t>1.7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Risiko 4 "Kinect: Menschliche Drehung" ist bereinigt. Zum jetztigen Projektzeitpunkt ist der Teaser, für welchen die Erkennung der Drehung relevant gewesen wäre, tief priorisiert. Er wird nicht mehr innerhalb des Zeitraums der BA implementiert werden können. </t>
   </si>
 </sst>
 </file>
@@ -455,17 +461,8 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -474,6 +471,15 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -698,7 +704,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A3:D10" totalsRowShown="0" headerRowDxfId="28" dataDxfId="27">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A3:D11" totalsRowShown="0" headerRowDxfId="28" dataDxfId="27">
   <tableColumns count="4">
     <tableColumn id="1" name="Datum" dataDxfId="26"/>
     <tableColumn id="2" name="Version" dataDxfId="25"/>
@@ -710,10 +716,10 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A3:J12" totalsRowCount="1" headerRowDxfId="21" dataDxfId="20" totalsRowDxfId="19">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A3:J12" totalsRowCount="1" headerRowDxfId="22" dataDxfId="21" totalsRowDxfId="20">
   <tableColumns count="10">
-    <tableColumn id="1" name="Nr." totalsRowLabel="Total" dataDxfId="18" totalsRowDxfId="9"/>
-    <tableColumn id="2" name="Risiko" dataDxfId="22" totalsRowDxfId="8"/>
+    <tableColumn id="1" name="Nr." totalsRowLabel="Total" dataDxfId="19" totalsRowDxfId="9"/>
+    <tableColumn id="2" name="Risiko" dataDxfId="18" totalsRowDxfId="8"/>
     <tableColumn id="3" name="Beschreibung" dataDxfId="17" totalsRowDxfId="7"/>
     <tableColumn id="4" name="W'keit des Eintretens [%]" dataDxfId="16" totalsRowDxfId="6"/>
     <tableColumn id="5" name="Schadens-potenzial [h]" totalsRowFunction="sum" dataDxfId="15" totalsRowDxfId="5"/>
@@ -1014,10 +1020,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1029,12 +1035,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="22.5" x14ac:dyDescent="0.3">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
       <c r="E1" s="9"/>
       <c r="F1" s="9"/>
       <c r="G1" s="9"/>
@@ -1158,6 +1164,20 @@
       </c>
       <c r="D10" s="4" t="s">
         <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="A11" s="11">
+        <v>41001</v>
+      </c>
+      <c r="B11" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -1177,8 +1197,8 @@
   <sheetPr codeName="Tabelle2"/>
   <dimension ref="A1:K18"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1197,18 +1217,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="22.5" x14ac:dyDescent="0.3">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
-      <c r="J1" s="19"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
     </row>
     <row r="3" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
@@ -1350,14 +1370,14 @@
         <v>27</v>
       </c>
       <c r="D7" s="4">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="E7" s="4">
         <v>30</v>
       </c>
       <c r="F7" s="4">
         <f t="shared" ref="F7" si="1">(D7/100)*E7</f>
-        <v>4.5</v>
+        <v>0</v>
       </c>
       <c r="G7" s="4" t="s">
         <v>30</v>
@@ -1368,7 +1388,9 @@
       <c r="I7" s="4">
         <v>2</v>
       </c>
-      <c r="J7" s="4"/>
+      <c r="J7" s="4">
+        <v>6</v>
+      </c>
     </row>
     <row r="8" spans="1:11" ht="105" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
@@ -1507,30 +1529,30 @@
       </c>
       <c r="F12" s="4">
         <f>SUBTOTAL(109,Table1[Reserven '[h']])</f>
-        <v>57.5</v>
+        <v>53</v>
       </c>
       <c r="G12" s="4"/>
       <c r="H12" s="4"/>
       <c r="I12" s="4"/>
       <c r="J12" s="4"/>
     </row>
-    <row r="13" spans="1:11" s="23" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" s="20" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="26" t="s">
         <v>62</v>
       </c>
       <c r="B13" s="27"/>
       <c r="C13" s="28"/>
-      <c r="D13" s="20"/>
-      <c r="E13" s="20"/>
-      <c r="F13" s="20">
+      <c r="D13" s="18"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="18">
         <f>25+8</f>
         <v>33</v>
       </c>
-      <c r="G13" s="20"/>
-      <c r="H13" s="20"/>
-      <c r="I13" s="20"/>
-      <c r="J13" s="20"/>
-      <c r="K13" s="24"/>
+      <c r="G13" s="18"/>
+      <c r="H13" s="18"/>
+      <c r="I13" s="18"/>
+      <c r="J13" s="18"/>
+      <c r="K13" s="21"/>
     </row>
     <row r="14" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A14" s="29" t="s">
@@ -1538,16 +1560,16 @@
       </c>
       <c r="B14" s="30"/>
       <c r="C14" s="31"/>
-      <c r="D14" s="20"/>
-      <c r="E14" s="20"/>
-      <c r="F14" s="20">
+      <c r="D14" s="18"/>
+      <c r="E14" s="18"/>
+      <c r="F14" s="18">
         <f>Table1[[#Totals],[Reserven '[h']]]-F13</f>
-        <v>24.5</v>
-      </c>
-      <c r="G14" s="20"/>
-      <c r="H14" s="20"/>
-      <c r="I14" s="20"/>
-      <c r="J14" s="20"/>
+        <v>20</v>
+      </c>
+      <c r="G14" s="18"/>
+      <c r="H14" s="18"/>
+      <c r="I14" s="18"/>
+      <c r="J14" s="18"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
@@ -1570,22 +1592,22 @@
       <c r="H16" s="1"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="21"/>
-      <c r="B17" s="21"/>
-      <c r="C17" s="21"/>
-      <c r="D17" s="22"/>
-      <c r="E17" s="22"/>
-      <c r="F17" s="25"/>
+      <c r="A17" s="24"/>
+      <c r="B17" s="24"/>
+      <c r="C17" s="24"/>
+      <c r="D17" s="19"/>
+      <c r="E17" s="19"/>
+      <c r="F17" s="22"/>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="21"/>
-      <c r="B18" s="21"/>
-      <c r="C18" s="21"/>
+      <c r="A18" s="24"/>
+      <c r="B18" s="24"/>
+      <c r="C18" s="24"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
-      <c r="F18" s="25"/>
+      <c r="F18" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>

<commit_message>
refs #689 Risikomanagement nachgeführt
Former-commit-id: 6ec2632e3275603f2c0de2747b3536222fcc9325
</commit_message>
<xml_diff>
--- a/doc/Bericht/05_Technischer Bericht/02_Projektmanagement/Risikomanagement.xlsx
+++ b/doc/Bericht/05_Technischer Bericht/02_Projektmanagement/Risikomanagement.xlsx
@@ -159,9 +159,6 @@
 Neue Risiken hinzugefügt (4,6,7), Schätzungen angepasst, Beschreibungen erweitert</t>
   </si>
   <si>
-    <t>Scrum, früher Prototyp, kleine Demoprogramme zu Beginn des Projektes. Kontinuierliche Überprüfung der Projektplanung und eventuelle Anpassung. Verantwortung für aktuellen Projektplan an einem Teammitglied zuweisen.</t>
-  </si>
-  <si>
     <t>Die Auflösung der Video Wall ist für das Lesen der Bachelor Posters ungenügend.</t>
   </si>
   <si>
@@ -238,6 +235,9 @@
   </si>
   <si>
     <t>Applikation so designen, dass die Performance nicht wichtig ist. Bsp: Geschickte Animationen, bei denen man nicht merkt, wenn sie langsam sind. Oder als Alternative: Auflösung verringern.</t>
+  </si>
+  <si>
+    <t>Scrum, früher Prototyp, kleine Demoprogramme zu Beginn des Projektes. Kontinuierliche Überprüfung der Projektplanung und eventuelle Anpassung.</t>
   </si>
 </sst>
 </file>
@@ -1133,10 +1133,10 @@
         <v>40970</v>
       </c>
       <c r="B7" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="C7" s="12" t="s">
         <v>49</v>
-      </c>
-      <c r="C7" s="12" t="s">
-        <v>50</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>22</v>
@@ -1147,10 +1147,10 @@
         <v>40976</v>
       </c>
       <c r="B8" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="C8" s="12" t="s">
         <v>51</v>
-      </c>
-      <c r="C8" s="12" t="s">
-        <v>52</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>41</v>
@@ -1161,10 +1161,10 @@
         <v>40984</v>
       </c>
       <c r="B9" s="16" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>22</v>
@@ -1175,10 +1175,10 @@
         <v>40991</v>
       </c>
       <c r="B10" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="C10" s="12" t="s">
         <v>60</v>
-      </c>
-      <c r="C10" s="12" t="s">
-        <v>61</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>41</v>
@@ -1189,10 +1189,10 @@
         <v>41001</v>
       </c>
       <c r="B11" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="C11" s="12" t="s">
         <v>65</v>
-      </c>
-      <c r="C11" s="12" t="s">
-        <v>66</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>22</v>
@@ -1203,10 +1203,10 @@
         <v>41015</v>
       </c>
       <c r="B12" s="16" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D12" s="4" t="s">
         <v>41</v>
@@ -1229,8 +1229,8 @@
   <sheetPr codeName="Tabelle2"/>
   <dimension ref="A1:K19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1327,7 +1327,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>2</v>
       </c>
@@ -1341,14 +1341,14 @@
         <v>10</v>
       </c>
       <c r="E5" s="4">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="F5" s="4">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>4.5</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>46</v>
+        <v>72</v>
       </c>
       <c r="H5" s="4" t="s">
         <v>13</v>
@@ -1363,10 +1363,10 @@
         <v>3</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D6" s="4">
         <v>0</v>
@@ -1432,7 +1432,7 @@
         <v>23</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D8" s="4">
         <v>5</v>
@@ -1448,7 +1448,7 @@
         <v>24</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I8" s="4">
         <v>1</v>
@@ -1522,10 +1522,10 @@
         <v>8</v>
       </c>
       <c r="B11" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C11" s="4" t="s">
         <v>57</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>58</v>
       </c>
       <c r="D11" s="4">
         <v>100</v>
@@ -1538,10 +1538,10 @@
         <v>8</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I11" s="4">
         <v>5</v>
@@ -1555,10 +1555,10 @@
         <v>9</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D12" s="4">
         <v>10</v>
@@ -1571,10 +1571,10 @@
         <v>10</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I12" s="4">
         <v>7</v>
@@ -1590,11 +1590,11 @@
       <c r="D13" s="4"/>
       <c r="E13" s="4">
         <f>SUBTOTAL(109,Table1[Schadens-potenzial '[h']])</f>
-        <v>443</v>
+        <v>438</v>
       </c>
       <c r="F13" s="4">
         <f>SUBTOTAL(109,Table1[Reserven '[h']])</f>
-        <v>63</v>
+        <v>62.5</v>
       </c>
       <c r="G13" s="4"/>
       <c r="H13" s="4"/>
@@ -1609,7 +1609,7 @@
     </row>
     <row r="14" spans="1:11" s="20" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="26" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B14" s="27"/>
       <c r="C14" s="28"/>
@@ -1627,7 +1627,7 @@
     </row>
     <row r="15" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A15" s="29" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B15" s="30"/>
       <c r="C15" s="31"/>
@@ -1635,7 +1635,7 @@
       <c r="E15" s="18"/>
       <c r="F15" s="18">
         <f>Table1[[#Totals],[Reserven '[h']]]-F14</f>
-        <v>30</v>
+        <v>29.5</v>
       </c>
       <c r="G15" s="18"/>
       <c r="H15" s="18"/>

</xml_diff>

<commit_message>
refs #882 Video Wall -> HSR Videowall
Former-commit-id: 8a48938783782e414e6600840c3dc69b34ce1ced
</commit_message>
<xml_diff>
--- a/doc/Bericht/05_Technischer Bericht/02_Projektmanagement/Risikomanagement.xlsx
+++ b/doc/Bericht/05_Technischer Bericht/02_Projektmanagement/Risikomanagement.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="30" windowWidth="12390" windowHeight="11955" activeTab="1"/>
+    <workbookView xWindow="-15" yWindow="30" windowWidth="12390" windowHeight="11955"/>
   </bookViews>
   <sheets>
     <sheet name="Änderungsgeschichte" sheetId="3" r:id="rId1"/>
@@ -89,12 +89,6 @@
     <t>DT</t>
   </si>
   <si>
-    <t>Auflösung der Video Wall ungenügend</t>
-  </si>
-  <si>
-    <t>Suchen einer Lösung für die Erstellung der Video Wall, bei der jeder einzelne Monitor Full HD ist.</t>
-  </si>
-  <si>
     <t>Frühe Anfrage, frühe Abklärungen durch Markus Stolze / Schulleitung.</t>
   </si>
   <si>
@@ -150,18 +144,12 @@
   </si>
   <si>
     <t>1.2</t>
-  </si>
-  <si>
-    <t>Die Hardware für die Video Wall kann nicht  rechtzeitig geliefert werden.</t>
   </si>
   <si>
     <t>Risiko 1 ist eingetreten: HW wird nicht rechtzeitig geliefert. Deshalb muss alternatives Testsetup evaluiert werden (Schaden: 25h).
 Neue Risiken hinzugefügt (4,6,7), Schätzungen angepasst, Beschreibungen erweitert</t>
   </si>
   <si>
-    <t>Die Auflösung der Video Wall ist für das Lesen der Bachelor Posters ungenügend.</t>
-  </si>
-  <si>
     <t>Darstellung der Poster in einer Grösse, die gut lesbar ist. Usability Tests müssen wiederholt werden. Alternative (2h Aufwand): Zu kleine Texte / Dokumente dürfen nicht hochgeladen / angezeigt werden (Constraint einführen).</t>
   </si>
   <si>
@@ -178,9 +166,6 @@
   </si>
   <si>
     <t>1.5</t>
-  </si>
-  <si>
-    <t>Kinect erkennt Menschen nicht, die sich parallel zur Wand ausgerichtet vor der Video Wall bewegen.</t>
   </si>
   <si>
     <t>Kinect: Erkennung von der Seite</t>
@@ -287,6 +272,21 @@
   </si>
   <si>
     <t>1.15</t>
+  </si>
+  <si>
+    <t>Die Hardware für die Videowall kann nicht  rechtzeitig geliefert werden.</t>
+  </si>
+  <si>
+    <t>Kinect erkennt Menschen nicht, die sich parallel zur Wand ausgerichtet vor der Videowall bewegen.</t>
+  </si>
+  <si>
+    <t>Auflösung der Videowall ungenügend</t>
+  </si>
+  <si>
+    <t>Die Auflösung der Videowall ist für das Lesen der Bachelor Posters ungenügend.</t>
+  </si>
+  <si>
+    <t>Suchen einer Lösung für die Erstellung der Videowall, bei der jeder einzelne Monitor Full HD ist.</t>
   </si>
 </sst>
 </file>
@@ -590,10 +590,10 @@
     </xf>
   </cellXfs>
   <cellStyles count="4">
-    <cellStyle name="20 % - Akzent4" xfId="3" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="Akzent4" xfId="2" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
-    <cellStyle name="Überschrift" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="3" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="2" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="36">
     <dxf>
@@ -823,9 +823,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Larissa">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -863,7 +863,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Larissa">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -935,7 +935,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Larissa">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1111,11 +1111,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.5703125" customWidth="1"/>
     <col min="2" max="2" width="10.140625" style="17" bestFit="1" customWidth="1"/>
@@ -1162,7 +1162,7 @@
         <v>40962</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>10</v>
@@ -1179,10 +1179,10 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -1190,13 +1190,13 @@
         <v>40970</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -1204,10 +1204,10 @@
         <v>40970</v>
       </c>
       <c r="B7" s="16" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>22</v>
@@ -1218,13 +1218,13 @@
         <v>40976</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -1232,10 +1232,10 @@
         <v>40984</v>
       </c>
       <c r="B9" s="16" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>22</v>
@@ -1246,13 +1246,13 @@
         <v>40991</v>
       </c>
       <c r="B10" s="16" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -1260,10 +1260,10 @@
         <v>41001</v>
       </c>
       <c r="B11" s="16" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>22</v>
@@ -1274,13 +1274,13 @@
         <v>41015</v>
       </c>
       <c r="B12" s="16" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -1288,10 +1288,10 @@
         <v>41029</v>
       </c>
       <c r="B13" s="16" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="D13" s="4" t="s">
         <v>22</v>
@@ -1302,13 +1302,13 @@
         <v>41036</v>
       </c>
       <c r="B14" s="16" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -1316,13 +1316,13 @@
         <v>41036</v>
       </c>
       <c r="B15" s="16" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -1330,13 +1330,13 @@
         <v>41038</v>
       </c>
       <c r="B16" s="16" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -1344,10 +1344,10 @@
         <v>41044</v>
       </c>
       <c r="B17" s="16" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="D17" s="4" t="s">
         <v>22</v>
@@ -1358,13 +1358,13 @@
         <v>41047</v>
       </c>
       <c r="B18" s="16" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -1372,13 +1372,13 @@
         <v>41057</v>
       </c>
       <c r="B19" s="16" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="C19" s="12" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -1398,11 +1398,11 @@
   <sheetPr codeName="Tabelle2"/>
   <dimension ref="A1:K20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16:C16"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.42578125" customWidth="1"/>
     <col min="2" max="2" width="14.7109375" customWidth="1"/>
@@ -1471,7 +1471,7 @@
         <v>21</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>44</v>
+        <v>84</v>
       </c>
       <c r="D4" s="4">
         <v>100</v>
@@ -1484,10 +1484,10 @@
         <v>25</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="I4" s="4">
         <v>1</v>
@@ -1496,7 +1496,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>2</v>
       </c>
@@ -1517,7 +1517,7 @@
         <v>4.5</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="H5" s="4" t="s">
         <v>13</v>
@@ -1532,10 +1532,10 @@
         <v>3</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>53</v>
+        <v>85</v>
       </c>
       <c r="D6" s="4">
         <v>0</v>
@@ -1548,10 +1548,10 @@
         <v>0</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="I6" s="4">
         <v>1</v>
@@ -1565,10 +1565,10 @@
         <v>4</v>
       </c>
       <c r="B7" s="23" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C7" s="23" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D7" s="23">
         <v>0</v>
@@ -1581,10 +1581,10 @@
         <v>0</v>
       </c>
       <c r="G7" s="23" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="H7" s="23" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="I7" s="23">
         <v>2</v>
@@ -1599,10 +1599,10 @@
         <v>5</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>23</v>
+        <v>86</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>46</v>
+        <v>87</v>
       </c>
       <c r="D8" s="4">
         <v>5</v>
@@ -1615,10 +1615,10 @@
         <v>3</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>24</v>
+        <v>88</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="I8" s="4">
         <v>1</v>
@@ -1630,10 +1630,10 @@
         <v>6</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D9" s="4">
         <v>100</v>
@@ -1646,10 +1646,10 @@
         <v>6</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="I9" s="4">
         <v>2</v>
@@ -1663,10 +1663,10 @@
         <v>7</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D10" s="4">
         <v>10</v>
@@ -1679,10 +1679,10 @@
         <v>6</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="I10" s="4">
         <v>2</v>
@@ -1694,10 +1694,10 @@
         <v>8</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="D11" s="4">
         <v>100</v>
@@ -1710,10 +1710,10 @@
         <v>8</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="I11" s="4">
         <v>5</v>
@@ -1727,10 +1727,10 @@
         <v>9</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="D12" s="4">
         <v>100</v>
@@ -1743,10 +1743,10 @@
         <v>10</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="I12" s="4">
         <v>7</v>
@@ -1760,10 +1760,10 @@
         <v>10</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="D13" s="4">
         <v>60</v>
@@ -1776,10 +1776,10 @@
         <v>24</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="I13" s="4">
         <v>11</v>
@@ -1814,7 +1814,7 @@
     </row>
     <row r="15" spans="1:11" s="20" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="29" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="B15" s="30"/>
       <c r="C15" s="31"/>
@@ -1832,7 +1832,7 @@
     </row>
     <row r="16" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A16" s="32" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="B16" s="33"/>
       <c r="C16" s="34"/>

</xml_diff>